<commit_message>
feature added import information about model
</commit_message>
<xml_diff>
--- a/matriz_de_confusao/matriz_excel.xlsx
+++ b/matriz_de_confusao/matriz_excel.xlsx
@@ -660,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -669,7 +669,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -708,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T3" t="n">
         <v>0</v>
@@ -723,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3" t="n">
         <v>0</v>
@@ -836,7 +836,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -872,10 +872,10 @@
         <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5" t="n">
         <v>0</v>
@@ -893,7 +893,7 @@
         <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="n">
         <v>0</v>
@@ -915,7 +915,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -924,7 +924,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -1009,10 +1009,10 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1027,7 +1027,7 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
@@ -1054,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V7" t="n">
         <v>0</v>
@@ -1100,7 +1100,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -1118,7 +1118,7 @@
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8" t="n">
         <v>0</v>
@@ -1136,7 +1136,7 @@
         <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" t="n">
         <v>0</v>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="n">
         <v>0</v>
@@ -1203,7 +1203,7 @@
         <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9" t="n">
         <v>0</v>
@@ -1218,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9" t="n">
         <v>0</v>
@@ -1361,10 +1361,10 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -1428,7 +1428,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -1452,13 +1452,13 @@
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12" t="n">
         <v>0</v>
@@ -1467,13 +1467,13 @@
         <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12" t="n">
         <v>0</v>
       </c>
       <c r="S12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T12" t="n">
         <v>0</v>
@@ -1491,7 +1491,7 @@
         <v>1</v>
       </c>
       <c r="Y12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z12" t="n">
         <v>0</v>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
@@ -1561,7 +1561,7 @@
         <v>0</v>
       </c>
       <c r="T13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U13" t="n">
         <v>0</v>
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -1658,7 +1658,7 @@
         <v>0</v>
       </c>
       <c r="X14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y14" t="n">
         <v>0</v>
@@ -1695,7 +1695,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -1707,7 +1707,7 @@
         <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15" t="n">
         <v>0</v>
@@ -1728,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="S15" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T15" t="n">
         <v>0</v>
@@ -1768,7 +1768,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -1780,37 +1780,37 @@
         <v>0</v>
       </c>
       <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
         <v>2</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0</v>
-      </c>
-      <c r="P16" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>0</v>
-      </c>
-      <c r="R16" t="n">
-        <v>3</v>
       </c>
       <c r="S16" t="n">
         <v>0</v>
@@ -1847,7 +1847,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -1892,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R17" t="n">
         <v>0</v>
@@ -1950,7 +1950,7 @@
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -1968,7 +1968,7 @@
         <v>0</v>
       </c>
       <c r="N18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O18" t="n">
         <v>0</v>
@@ -1980,10 +1980,10 @@
         <v>0</v>
       </c>
       <c r="R18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T18" t="n">
         <v>0</v>
@@ -2102,7 +2102,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -2120,7 +2120,7 @@
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
@@ -2153,10 +2153,10 @@
         <v>0</v>
       </c>
       <c r="S20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U20" t="n">
         <v>0</v>
@@ -2281,7 +2281,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -2308,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="N22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O22" t="n">
         <v>0</v>
@@ -2332,13 +2332,13 @@
         <v>0</v>
       </c>
       <c r="V22" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W22" t="n">
         <v>0</v>
       </c>
       <c r="X22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y22" t="n">
         <v>0</v>
@@ -2369,7 +2369,7 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
@@ -2393,7 +2393,7 @@
         <v>0</v>
       </c>
       <c r="N23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O23" t="n">
         <v>0</v>
@@ -2423,13 +2423,13 @@
         <v>5</v>
       </c>
       <c r="X23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y23" t="n">
         <v>0</v>
       </c>
       <c r="Z23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA23" t="n">
         <v>0</v>
@@ -2460,7 +2460,7 @@
         <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
@@ -2478,7 +2478,7 @@
         <v>0</v>
       </c>
       <c r="N24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O24" t="n">
         <v>0</v>
@@ -2493,7 +2493,7 @@
         <v>0</v>
       </c>
       <c r="S24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T24" t="n">
         <v>0</v>
@@ -2508,7 +2508,7 @@
         <v>0</v>
       </c>
       <c r="X24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Y24" t="n">
         <v>0</v>
@@ -2527,7 +2527,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
@@ -2596,7 +2596,7 @@
         <v>0</v>
       </c>
       <c r="Y25" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Z25" t="n">
         <v>0</v>
@@ -2681,10 +2681,10 @@
         <v>0</v>
       </c>
       <c r="Y26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA26" t="n">
         <v>0</v>
@@ -2697,7 +2697,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -2724,7 +2724,7 @@
         <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27" t="n">
         <v>0</v>
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
       <c r="AA27" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix added comment for function
</commit_message>
<xml_diff>
--- a/matriz_de_confusao/matriz_excel.xlsx
+++ b/matriz_de_confusao/matriz_excel.xlsx
@@ -572,10 +572,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -660,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -669,7 +669,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -708,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T3" t="n">
         <v>0</v>
@@ -723,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="n">
         <v>0</v>
@@ -745,10 +745,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -830,13 +830,13 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -872,10 +872,10 @@
         <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
         <v>0</v>
@@ -893,7 +893,7 @@
         <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y5" t="n">
         <v>0</v>
@@ -915,7 +915,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -924,7 +924,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -936,7 +936,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
@@ -1009,10 +1009,10 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1027,7 +1027,7 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
@@ -1054,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7" t="n">
         <v>0</v>
@@ -1085,7 +1085,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -1100,7 +1100,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -1112,7 +1112,7 @@
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" t="n">
         <v>0</v>
@@ -1136,7 +1136,7 @@
         <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" t="n">
         <v>0</v>
@@ -1170,7 +1170,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -1188,7 +1188,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -1203,10 +1203,10 @@
         <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9" t="n">
         <v>0</v>
@@ -1218,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T9" t="n">
         <v>0</v>
@@ -1276,10 +1276,10 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
         <v>0</v>
@@ -1361,10 +1361,10 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -1452,7 +1452,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
@@ -1467,13 +1467,13 @@
         <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R12" t="n">
         <v>0</v>
       </c>
       <c r="S12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T12" t="n">
         <v>0</v>
@@ -1488,10 +1488,10 @@
         <v>0</v>
       </c>
       <c r="X12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z12" t="n">
         <v>0</v>
@@ -1531,7 +1531,7 @@
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
@@ -1540,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="N13" t="n">
         <v>0</v>
@@ -1561,7 +1561,7 @@
         <v>0</v>
       </c>
       <c r="T13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U13" t="n">
         <v>0</v>
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -1628,7 +1628,7 @@
         <v>0</v>
       </c>
       <c r="N14" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="O14" t="n">
         <v>0</v>
@@ -1643,7 +1643,7 @@
         <v>0</v>
       </c>
       <c r="S14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T14" t="n">
         <v>0</v>
@@ -1658,7 +1658,7 @@
         <v>0</v>
       </c>
       <c r="X14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y14" t="n">
         <v>0</v>
@@ -1680,7 +1680,7 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -1713,10 +1713,10 @@
         <v>0</v>
       </c>
       <c r="N15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O15" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P15" t="n">
         <v>0</v>
@@ -1728,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="S15" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T15" t="n">
         <v>0</v>
@@ -1746,7 +1746,7 @@
         <v>0</v>
       </c>
       <c r="Y15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z15" t="n">
         <v>0</v>
@@ -1771,7 +1771,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -1780,7 +1780,7 @@
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -1828,7 +1828,7 @@
         <v>0</v>
       </c>
       <c r="X16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y16" t="n">
         <v>0</v>
@@ -1862,7 +1862,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1892,13 +1892,13 @@
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="R17" t="n">
         <v>0</v>
       </c>
       <c r="S17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T17" t="n">
         <v>0</v>
@@ -1950,7 +1950,7 @@
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -1968,7 +1968,7 @@
         <v>0</v>
       </c>
       <c r="N18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O18" t="n">
         <v>0</v>
@@ -1980,7 +1980,7 @@
         <v>0</v>
       </c>
       <c r="R18" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S18" t="n">
         <v>0</v>
@@ -1998,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="X18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y18" t="n">
         <v>0</v>
@@ -2017,10 +2017,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -2038,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
@@ -2068,7 +2068,7 @@
         <v>0</v>
       </c>
       <c r="S19" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T19" t="n">
         <v>0</v>
@@ -2120,7 +2120,7 @@
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
@@ -2156,7 +2156,7 @@
         <v>0</v>
       </c>
       <c r="T20" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U20" t="n">
         <v>0</v>
@@ -2202,7 +2202,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -2211,7 +2211,7 @@
         <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" t="n">
         <v>0</v>
@@ -2244,7 +2244,7 @@
         <v>0</v>
       </c>
       <c r="U21" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="V21" t="n">
         <v>0</v>
@@ -2308,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="N22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O22" t="n">
         <v>0</v>
@@ -2320,7 +2320,7 @@
         <v>0</v>
       </c>
       <c r="R22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S22" t="n">
         <v>0</v>
@@ -2332,7 +2332,7 @@
         <v>0</v>
       </c>
       <c r="V22" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="W22" t="n">
         <v>0</v>
@@ -2360,7 +2360,7 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -2369,7 +2369,7 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
@@ -2393,7 +2393,7 @@
         <v>0</v>
       </c>
       <c r="N23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O23" t="n">
         <v>0</v>
@@ -2402,7 +2402,7 @@
         <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R23" t="n">
         <v>0</v>
@@ -2420,7 +2420,7 @@
         <v>0</v>
       </c>
       <c r="W23" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="X23" t="n">
         <v>0</v>
@@ -2478,7 +2478,7 @@
         <v>0</v>
       </c>
       <c r="N24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O24" t="n">
         <v>0</v>
@@ -2493,7 +2493,7 @@
         <v>0</v>
       </c>
       <c r="S24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T24" t="n">
         <v>0</v>
@@ -2508,7 +2508,7 @@
         <v>0</v>
       </c>
       <c r="X24" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="Y24" t="n">
         <v>0</v>
@@ -2527,7 +2527,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
@@ -2557,7 +2557,7 @@
         <v>0</v>
       </c>
       <c r="L25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M25" t="n">
         <v>0</v>
@@ -2596,7 +2596,7 @@
         <v>0</v>
       </c>
       <c r="Y25" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Z25" t="n">
         <v>0</v>
@@ -2627,7 +2627,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
@@ -2657,7 +2657,7 @@
         <v>0</v>
       </c>
       <c r="Q26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R26" t="n">
         <v>0</v>
@@ -2681,10 +2681,10 @@
         <v>0</v>
       </c>
       <c r="Y26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z26" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AA26" t="n">
         <v>0</v>
@@ -2697,7 +2697,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -2721,7 +2721,7 @@
         <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" t="n">
         <v>1</v>
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
       <c r="AA27" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>